<commit_message>
Fix sitemap URLs: Use Punycode domain (xn--selbstndig-schweiz-qtb.ch)
SEO Fix:
- Sitemap URLs now use Punycode (xn--selbstndig-schweiz-qtb.ch)
- Required for Google Search Console and SEO tools
- IndexNow host updated to Punycode version
- Environment variable updated

Technical:
- selbständig-schweiz.ch → xn--selbstndig-schweiz-qtb.ch
- Ensures compatibility with all SEO tools
- Fixes "Sitemap not found" error in GSC

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CONTENT-KALENDER-KOMPLETT.xlsx
+++ b/CONTENT-KALENDER-KOMPLETT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romanstalder/Dropbox/JETZT/01 CODE/selbstaendig-schweiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9B38C6-077A-5B44-ADC8-F82E4C2A596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB54BD39-46D4-534F-984B-565C822E3E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="22940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="358">
   <si>
     <t>Rank</t>
   </si>
@@ -1051,9 +1051,6 @@
     <t>Pillar page 10</t>
   </si>
   <si>
-    <t>selbständig machen in der schweiz</t>
-  </si>
-  <si>
     <t>generiert</t>
   </si>
   <si>
@@ -1073,6 +1070,30 @@
   </si>
   <si>
     <t>gmbh gründen schweiz</t>
+  </si>
+  <si>
+    <t>selbständig machen schweiz</t>
+  </si>
+  <si>
+    <t>selbständig als berater</t>
+  </si>
+  <si>
+    <t>selbständig als webdesigner</t>
+  </si>
+  <si>
+    <t>selbständig als fotograf</t>
+  </si>
+  <si>
+    <t>selbständig als schreiner</t>
+  </si>
+  <si>
+    <t>selbständig als elektriker</t>
+  </si>
+  <si>
+    <t>selbständig als programmierer</t>
+  </si>
+  <si>
+    <t>selbständig als treuhänder</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1183,6 +1204,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1487,10 +1512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J307"/>
+  <dimension ref="A1:K314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,7 +1533,7 @@
     <col min="10" max="10" width="9.33203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>333</v>
@@ -1548,7 +1574,7 @@
         <v>41</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1558,10 +1584,10 @@
         <v>37</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>334</v>
@@ -1570,7 +1596,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1580,10 +1606,10 @@
         <v>52</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>335</v>
@@ -1602,10 +1628,10 @@
         <v>16</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>336</v>
@@ -1614,7 +1640,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1624,10 +1650,10 @@
         <v>13</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>337</v>
@@ -1636,7 +1662,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1646,10 +1672,10 @@
         <v>48</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>338</v>
@@ -1658,7 +1684,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1668,10 +1694,10 @@
         <v>20</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>339</v>
@@ -1680,7 +1706,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1690,10 +1716,10 @@
         <v>146</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>340</v>
@@ -1712,10 +1738,10 @@
         <v>63</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>341</v>
@@ -1734,10 +1760,10 @@
         <v>37</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>342</v>
@@ -1746,7 +1772,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1756,586 +1782,640 @@
         <v>37</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="6">
         <v>2400</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="6">
         <v>10</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="6">
         <v>11.87</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="6">
         <v>81.5</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="J12" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K12" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="6">
         <v>1600</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="6">
         <v>13</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="6">
         <v>11.42</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="6">
         <v>69.8</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="J13" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K13" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="6">
         <v>4400</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="6">
         <v>24</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="6">
         <v>7.23</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="6">
         <v>64.5</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="J14" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K14" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="6">
         <v>6600</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="6">
         <v>26</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="6">
         <v>7.44</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="6">
         <v>62.4</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="J15" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K15" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="6">
         <v>6600</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="6">
         <v>30</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="6">
         <v>9.89</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="6">
         <v>62.3</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="J16" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K16" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>6</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="6">
         <v>1600</v>
       </c>
-      <c r="F17" s="2">
-        <v>14</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="F17" s="6">
+        <v>14</v>
+      </c>
+      <c r="G17" s="6">
         <v>6.84</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="6">
         <v>62.2</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="I17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K17" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>7</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="6">
         <v>1600</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="6">
         <v>13</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="6">
         <v>6.2</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="6">
         <v>62.1</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="J18" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K18" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>8</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="6">
         <v>140</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="6">
         <v>8</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="6">
         <v>11.96</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="6">
         <v>61.4</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="I19" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K19" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>9</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="6">
         <v>2900</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="6">
         <v>26</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="6">
         <v>6.96</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="6">
         <v>60.4</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="I20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K20" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>10</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="6">
         <v>170</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="6">
         <v>9</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="6">
         <v>9.93</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="6">
         <v>60.3</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="J21" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K21" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
         <v>11</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="6">
         <v>4400</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="6">
         <v>17</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="6">
         <v>0.73</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="6">
         <v>60.2</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="I22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K22" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>12</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>2900</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="6">
         <v>30</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="6">
         <v>8.85</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="6">
         <v>59.2</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="I23" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K23" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
         <v>13</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="6">
         <v>480</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="6">
         <v>13</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="6">
         <v>15.27</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="6">
         <v>58.5</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>14</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="J24" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K24" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>14</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="6">
         <v>2900</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="6">
         <v>20</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="6">
         <v>2.21</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="6">
         <v>58.4</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="I25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K25" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>15</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="6">
         <v>50</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="6">
         <v>10</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="6">
         <v>10.59</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="6">
         <v>58</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="I26" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K26" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>16</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="6">
         <v>1000</v>
       </c>
-      <c r="F27" s="2">
-        <v>14</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="F27" s="6">
+        <v>14</v>
+      </c>
+      <c r="G27" s="6">
         <v>7.66</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="6">
         <v>57.8</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="J27" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K27" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="6">
         <v>2400</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="6">
         <v>18</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="6">
         <v>2.75</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="6">
         <v>57</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="J28" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K28" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>18</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="6">
         <v>110</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="6">
         <v>6</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="6">
         <v>6.58</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="6">
         <v>56.8</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I29" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K29" s="15">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>19</v>
       </c>
@@ -2363,11 +2443,14 @@
       <c r="I30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K30" s="15">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>20</v>
       </c>
@@ -2395,11 +2478,14 @@
       <c r="I31" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J31" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K31" s="15">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>21</v>
       </c>
@@ -2427,11 +2513,14 @@
       <c r="I32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J32" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K32" s="15">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>22</v>
       </c>
@@ -2459,11 +2548,14 @@
       <c r="I33" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J33" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K33" s="15">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>23</v>
       </c>
@@ -2495,7 +2587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>24</v>
       </c>
@@ -2527,7 +2619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>25</v>
       </c>
@@ -2559,7 +2651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>26</v>
       </c>
@@ -2591,7 +2683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>27</v>
       </c>
@@ -2623,7 +2715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>28</v>
       </c>
@@ -2655,7 +2747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>29</v>
       </c>
@@ -2687,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>30</v>
       </c>
@@ -2719,7 +2811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>31</v>
       </c>
@@ -2751,7 +2843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>32</v>
       </c>
@@ -2783,7 +2875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>33</v>
       </c>
@@ -2815,7 +2907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>34</v>
       </c>
@@ -2847,7 +2939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>35</v>
       </c>
@@ -2879,7 +2971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>36</v>
       </c>
@@ -2911,7 +3003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>37</v>
       </c>
@@ -11135,7 +11227,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" s="5">
         <v>294</v>
       </c>
@@ -11167,7 +11259,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" s="5">
         <v>295</v>
       </c>
@@ -11199,7 +11291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" s="5">
         <v>296</v>
       </c>
@@ -11231,7 +11323,169 @@
         <v>14</v>
       </c>
     </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D308" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="E308" s="6">
+        <v>10</v>
+      </c>
+      <c r="F308" s="6">
+        <v>35</v>
+      </c>
+      <c r="G308" s="6">
+        <v>0</v>
+      </c>
+      <c r="I308" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J308" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K308" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D309" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="E309" s="6">
+        <v>10</v>
+      </c>
+      <c r="F309" s="6">
+        <v>29</v>
+      </c>
+      <c r="G309" s="6">
+        <v>0</v>
+      </c>
+      <c r="I309" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J309" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K309" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D310" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="E310" s="6">
+        <v>10</v>
+      </c>
+      <c r="F310" s="6">
+        <v>13</v>
+      </c>
+      <c r="G310" s="6">
+        <v>0</v>
+      </c>
+      <c r="I310" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J310" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K310" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D311" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="E311" s="6">
+        <v>0</v>
+      </c>
+      <c r="F311" s="6">
+        <v>12</v>
+      </c>
+      <c r="G311" s="6">
+        <v>0</v>
+      </c>
+      <c r="I311" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J311" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K311" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D312" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="E312" s="6">
+        <v>10</v>
+      </c>
+      <c r="F312" s="6">
+        <v>16</v>
+      </c>
+      <c r="G312" s="6">
+        <v>0</v>
+      </c>
+      <c r="I312" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J312" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K312" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D313" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="E313" s="6">
+        <v>10</v>
+      </c>
+      <c r="F313" s="6">
+        <v>13</v>
+      </c>
+      <c r="G313" s="6">
+        <v>0</v>
+      </c>
+      <c r="I313" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J313" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K313" s="15">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D314" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E314" s="6">
+        <v>0</v>
+      </c>
+      <c r="F314" s="6">
+        <v>12</v>
+      </c>
+      <c r="G314" s="6">
+        <v>0</v>
+      </c>
+      <c r="I314" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J314" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K314" s="15">
+        <v>45998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>